<commit_message>
added JRS/RTI Google tests
</commit_message>
<xml_diff>
--- a/docs/my-6502-emulator.xlsx
+++ b/docs/my-6502-emulator.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
   <si>
     <t xml:space="preserve">Topic</t>
   </si>
@@ -63,12 +63,11 @@
 - Invaluable for debugging</t>
   </si>
   <si>
-    <t xml:space="preserve">Stack ops &amp; interrupts</t>
+    <t xml:space="preserve">Stack ops</t>
   </si>
   <si>
     <t xml:space="preserve">- PHA, PLA
-- PHP, PLP
-- BRK, RTI</t>
+- PHP, PLP</t>
   </si>
   <si>
     <t xml:space="preserve">Arithmetic (ADC, SBC)</t>
@@ -96,6 +95,12 @@
   </si>
   <si>
     <t xml:space="preserve">Self-test ROM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Google Test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://github.com/google/googletest.git</t>
   </si>
 </sst>
 </file>
@@ -105,11 +110,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -125,6 +131,13 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -169,20 +182,28 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -309,10 +330,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
+      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -375,15 +396,15 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="24.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F6" s="0"/>
-      <c r="G6" s="0"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
     </row>
     <row r="7" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
@@ -395,8 +416,8 @@
       <c r="C7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F7" s="0"/>
-      <c r="G7" s="0"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
     </row>
     <row r="8" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
@@ -405,8 +426,8 @@
       <c r="B8" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F8" s="0"/>
-      <c r="G8" s="0"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
     </row>
     <row r="9" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
@@ -415,8 +436,8 @@
       <c r="B9" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F9" s="0"/>
-      <c r="G9" s="0"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
@@ -428,7 +449,21 @@
         <v>21</v>
       </c>
     </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B12" r:id="rId1" display="https://github.com/google/googletest.git"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>